<commit_message>
Fin carnet d'adresses DAO
</commit_message>
<xml_diff>
--- a/Ressources-Tp-DAO/CarnetAdressesDAO/carnetadr_bdd/BDD.xlsx
+++ b/Ressources-Tp-DAO/CarnetAdressesDAO/carnetadr_bdd/BDD.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="28">
   <si>
     <t>idPers</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>NewPrenom</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>rue</t>
+  </si>
+  <si>
+    <t>ville</t>
+  </si>
+  <si>
+    <t>newrue</t>
+  </si>
+  <si>
+    <t>newville</t>
   </si>
 </sst>
 </file>
@@ -456,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB325CE-F8DD-A94D-814B-38416559F980}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -509,20 +524,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -530,7 +531,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D581E5AE-91FC-5243-B7F8-A7C45E3B6C42}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -598,19 +599,36 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B4" t="n">
         <v>10.0</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>97000.0</v>
+        <v>86000.0</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="n">
+        <v>87000.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>